<commit_message>
CHG: Riskmanagement und Environment ausgefüllt
</commit_message>
<xml_diff>
--- a/Documentation/Week5/RiskManagement.xlsx
+++ b/Documentation/Week5/RiskManagement.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>Identified</t>
   </si>
@@ -34,15 +34,103 @@
   </si>
   <si>
     <t>risk factor</t>
+  </si>
+  <si>
+    <t>Ausfall eines Teammitglieds</t>
+  </si>
+  <si>
+    <t>Datenverlust</t>
+  </si>
+  <si>
+    <t>Ausfall eines zur Entwicklung benötigten Gerätes</t>
+  </si>
+  <si>
+    <t>Ausfall des JIRA Servers</t>
+  </si>
+  <si>
+    <t>Zeitmangel durch andere Projekte/Vorlesungen</t>
+  </si>
+  <si>
+    <t>mangelndes Fachwissen</t>
+  </si>
+  <si>
+    <t>fehlende Testgeräte (Tablet)</t>
+  </si>
+  <si>
+    <t>zu großer Scope</t>
+  </si>
+  <si>
+    <t>Konflikte zwischen MAC und Windows</t>
+  </si>
+  <si>
+    <t>fehlerhafte (Zeit-)Planung</t>
+  </si>
+  <si>
+    <t>großzügig planen, Erfahrungswerte vom Anfang des Projekts für spätere Schätzungen nutzen (Function Points)</t>
+  </si>
+  <si>
+    <t>genügend Zeit für andere Projekte einplanen</t>
+  </si>
+  <si>
+    <t>"Mindest-"Scope festlegen, sodass das Spiel funktionsfähig ist, entsprechende Priorisierung der Use Cases</t>
+  </si>
+  <si>
+    <t>Zeit für Tutorials einplanen</t>
+  </si>
+  <si>
+    <t>sofortige Kommunikation, eventuell HomeOffice und Umverteilung der Aufgaben</t>
+  </si>
+  <si>
+    <t>Emulator und Smartphone nutzen</t>
+  </si>
+  <si>
+    <t>häufige Synchronisation mit Git Hub Repository</t>
+  </si>
+  <si>
+    <t>MS Project-Datei mit Taskliste nutzen, Kommunikation über Skype</t>
+  </si>
+  <si>
+    <t>Ersatzlaptop</t>
+  </si>
+  <si>
+    <t>Reviews auf beiden Betriebssystemen</t>
+  </si>
+  <si>
+    <t>Christiane</t>
+  </si>
+  <si>
+    <t>Yvonne</t>
+  </si>
+  <si>
+    <t>Janina</t>
+  </si>
+  <si>
+    <t>Risikomanagement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -78,25 +166,58 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="8">
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -109,15 +230,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:F10" totalsRowShown="0">
-  <autoFilter ref="A1:F10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A3:F13" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A3:F13"/>
+  <sortState ref="A2:F11">
+    <sortCondition descending="1" ref="B1:B11"/>
+  </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="Identified" dataDxfId="0"/>
-    <tableColumn id="2" name="risk factor"/>
-    <tableColumn id="3" name="prob of occurrence"/>
-    <tableColumn id="4" name="damage"/>
-    <tableColumn id="5" name="mitigation strategy"/>
-    <tableColumn id="6" name="person in charge"/>
+    <tableColumn id="1" name="Identified" dataDxfId="4"/>
+    <tableColumn id="2" name="risk factor" dataDxfId="3">
+      <calculatedColumnFormula>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="prob of occurrence" dataDxfId="2"/>
+    <tableColumn id="4" name="damage" dataDxfId="0"/>
+    <tableColumn id="5" name="mitigation strategy" dataDxfId="1"/>
+    <tableColumn id="6" name="person in charge" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -410,65 +536,266 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="20.7109375" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4">
+        <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
+        <v>6.4</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="D4" s="4">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4">
+        <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
+        <v>5.6</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="D5" s="4">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4">
+        <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
+        <v>5.2</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.65</v>
+      </c>
+      <c r="D6" s="4">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4">
+        <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
+        <v>4.5</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="4">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4">
+        <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
+        <v>3.5</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="4">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4">
+        <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="D9" s="4">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4">
+        <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="D10" s="4">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4">
+        <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
+        <v>0.2</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4">
+        <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="D12" s="4">
+        <v>3</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="4">
+        <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
+        <v>0.05</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="97" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>